<commit_message>
Conception traj pour homologation
</commit_message>
<xml_diff>
--- a/Dev_uCOS-II/Oufff2011/Conception/Calculs trajectoires.xlsx
+++ b/Dev_uCOS-II/Oufff2011/Conception/Calculs trajectoires.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Caractéristiques robot</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>case 1</t>
+  </si>
+  <si>
+    <t>ATTENTION : L'angle est en radian</t>
   </si>
 </sst>
 </file>
@@ -129,16 +132,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,19 +253,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>-183</c:v>
+                  <c:v>729.40054095713822</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-183</c:v>
+                  <c:v>1570.5994590428618</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-183</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-183</c:v>
+                  <c:v>2270.5994590428618</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-183</c:v>
+                  <c:v>1429.4005409571382</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-183</c:v>
@@ -330,19 +337,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>420.59945904286178</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>279.40054095713822</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>420.59945904286178</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>279.40054095713822</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -417,11 +424,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="127966528"/>
-        <c:axId val="139444224"/>
+        <c:axId val="81174912"/>
+        <c:axId val="81176448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127966528"/>
+        <c:axId val="81174912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3000"/>
@@ -434,14 +441,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139444224"/>
+        <c:crossAx val="81176448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="500"/>
-        <c:minorUnit val="100"/>
+        <c:majorUnit val="150"/>
+        <c:minorUnit val="150"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139444224"/>
+        <c:axId val="81176448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100"/>
@@ -454,10 +461,10 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127966528"/>
+        <c:crossAx val="81174912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="500"/>
+        <c:majorUnit val="150"/>
         <c:minorUnit val="100"/>
       </c:valAx>
     </c:plotArea>
@@ -486,7 +493,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -497,7 +504,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9316983" cy="6076293"/>
+    <xdr:ext cx="9301574" cy="6079537"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
@@ -810,7 +817,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,10 +875,10 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -974,289 +981,318 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1">
-        <f>A3-Paramètres!$B$6*COS(C3)</f>
-        <v>-183</v>
+        <f>A3-Paramètres!$B$6*COS(C3*PI()/180 )</f>
+        <v>729.40054095713822</v>
       </c>
       <c r="E3" s="1">
-        <f>B3-Paramètres!$B$6*SIN(C3)</f>
-        <v>0</v>
+        <f>B3-Paramètres!$B$6*SIN(C3*PI()/180)</f>
+        <v>420.59945904286178</v>
       </c>
       <c r="F3" s="1">
-        <f>C3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F3:F27" si="0">C3</f>
+        <v>135</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+        <v>1700</v>
+      </c>
+      <c r="B4" s="1">
+        <v>150</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-45</v>
+      </c>
       <c r="D4" s="1">
-        <f>A4-Paramètres!$B$6*COS(C4)</f>
-        <v>-183</v>
+        <f>A4-Paramètres!$B$6*COS(C4*PI()/180 )</f>
+        <v>1570.5994590428618</v>
       </c>
       <c r="E4" s="1">
-        <f>B4-Paramètres!$B$6*SIN(C4)</f>
-        <v>0</v>
+        <f>B4-Paramètres!$B$6*SIN(C4*PI()/180)</f>
+        <v>279.40054095713822</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F27" si="0">C4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <f>A5-Paramètres!$B$6*COS(C5)</f>
+        <f>A5-Paramètres!$B$6*COS(C5*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E5" s="1">
-        <f>B5-Paramètres!$B$6*SIN(C5)</f>
+        <f>B5-Paramètres!$B$6*SIN(C5*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+        <f t="shared" ref="F4:F27" si="1">C5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2400</v>
+      </c>
+      <c r="B6" s="1">
+        <v>550</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45</v>
+      </c>
       <c r="D6" s="1">
-        <f>A6-Paramètres!$B$6*COS(C6)</f>
-        <v>-183</v>
+        <f>A6-Paramètres!$B$6*COS(C6*PI()/180 )</f>
+        <v>2270.5994590428618</v>
       </c>
       <c r="E6" s="1">
-        <f>B6-Paramètres!$B$6*SIN(C6)</f>
-        <v>0</v>
+        <f>B6-Paramètres!$B$6*SIN(C6*PI()/180)</f>
+        <v>420.59945904286178</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+        <f t="shared" ref="F6:F27" si="2">C6</f>
+        <v>45</v>
+      </c>
+      <c r="H6" s="6">
+        <f>3000-D6</f>
+        <v>729.40054095713822</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1300</v>
+      </c>
+      <c r="B7" s="1">
+        <v>150</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-135</v>
+      </c>
       <c r="D7" s="1">
-        <f>A7-Paramètres!$B$6*COS(C7)</f>
-        <v>-183</v>
+        <f>A7-Paramètres!$B$6*COS(C7*PI()/180 )</f>
+        <v>1429.4005409571382</v>
       </c>
       <c r="E7" s="1">
-        <f>B7-Paramètres!$B$6*SIN(C7)</f>
-        <v>0</v>
+        <f>B7-Paramètres!$B$6*SIN(C7*PI()/180)</f>
+        <v>279.40054095713822</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-135</v>
+      </c>
+      <c r="H7" s="6">
+        <f>3000-D7</f>
+        <v>1570.5994590428618</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <f>A8-Paramètres!$B$6*COS(C8)</f>
+        <f>A8-Paramètres!$B$6*COS(C8*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E8" s="1">
-        <f>B8-Paramètres!$B$6*SIN(C8)</f>
+        <f>B8-Paramètres!$B$6*SIN(C8*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
-        <f>A9-Paramètres!$B$6*COS(C9)</f>
+        <f>A9-Paramètres!$B$6*COS(C9*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E9" s="1">
-        <f>B9-Paramètres!$B$6*SIN(C9)</f>
+        <f>B9-Paramètres!$B$6*SIN(C9*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
-        <f>A10-Paramètres!$B$6*COS(C10)</f>
+        <f>A10-Paramètres!$B$6*COS(C10*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E10" s="1">
-        <f>B10-Paramètres!$B$6*SIN(C10)</f>
+        <f>B10-Paramètres!$B$6*SIN(C10*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
-        <f>A11-Paramètres!$B$6*COS(C11)</f>
+        <f>A11-Paramètres!$B$6*COS(C11*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E11" s="1">
-        <f>B11-Paramètres!$B$6*SIN(C11)</f>
+        <f>B11-Paramètres!$B$6*SIN(C11*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
-        <f>A12-Paramètres!$B$6*COS(C12)</f>
+        <f>A12-Paramètres!$B$6*COS(C12*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E12" s="1">
-        <f>B12-Paramètres!$B$6*SIN(C12)</f>
+        <f>B12-Paramètres!$B$6*SIN(C12*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
-        <f>A13-Paramètres!$B$6*COS(C13)</f>
+        <f>A13-Paramètres!$B$6*COS(C13*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E13" s="1">
-        <f>B13-Paramètres!$B$6*SIN(C13)</f>
+        <f>B13-Paramètres!$B$6*SIN(C13*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
-        <f>A14-Paramètres!$B$6*COS(C14)</f>
+        <f>A14-Paramètres!$B$6*COS(C14*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E14" s="1">
-        <f>B14-Paramètres!$B$6*SIN(C14)</f>
+        <f>B14-Paramètres!$B$6*SIN(C14*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
-        <f>A15-Paramètres!$B$6*COS(C15)</f>
+        <f>A15-Paramètres!$B$6*COS(C15*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E15" s="1">
-        <f>B15-Paramètres!$B$6*SIN(C15)</f>
+        <f>B15-Paramètres!$B$6*SIN(C15*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
-        <f>A16-Paramètres!$B$6*COS(C16)</f>
+        <f>A16-Paramètres!$B$6*COS(C16*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E16" s="1">
-        <f>B16-Paramètres!$B$6*SIN(C16)</f>
+        <f>B16-Paramètres!$B$6*SIN(C16*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1265,15 +1301,15 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
-        <f>A17-Paramètres!$B$6*COS(C17)</f>
+        <f>A17-Paramètres!$B$6*COS(C17*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E17" s="1">
-        <f>B17-Paramètres!$B$6*SIN(C17)</f>
+        <f>B17-Paramètres!$B$6*SIN(C17*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1282,15 +1318,15 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
-        <f>A18-Paramètres!$B$6*COS(C18)</f>
+        <f>A18-Paramètres!$B$6*COS(C18*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E18" s="1">
-        <f>B18-Paramètres!$B$6*SIN(C18)</f>
+        <f>B18-Paramètres!$B$6*SIN(C18*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1299,15 +1335,15 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
-        <f>A19-Paramètres!$B$6*COS(C19)</f>
+        <f>A19-Paramètres!$B$6*COS(C19*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E19" s="1">
-        <f>B19-Paramètres!$B$6*SIN(C19)</f>
+        <f>B19-Paramètres!$B$6*SIN(C19*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1316,15 +1352,15 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
-        <f>A20-Paramètres!$B$6*COS(C20)</f>
+        <f>A20-Paramètres!$B$6*COS(C20*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E20" s="1">
-        <f>B20-Paramètres!$B$6*SIN(C20)</f>
+        <f>B20-Paramètres!$B$6*SIN(C20*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1333,15 +1369,15 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <f>A21-Paramètres!$B$6*COS(C21)</f>
+        <f>A21-Paramètres!$B$6*COS(C21*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E21" s="1">
-        <f>B21-Paramètres!$B$6*SIN(C21)</f>
+        <f>B21-Paramètres!$B$6*SIN(C21*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1350,15 +1386,15 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
-        <f>A22-Paramètres!$B$6*COS(C22)</f>
+        <f>A22-Paramètres!$B$6*COS(C22*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E22" s="1">
-        <f>B22-Paramètres!$B$6*SIN(C22)</f>
+        <f>B22-Paramètres!$B$6*SIN(C22*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1367,15 +1403,15 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
-        <f>A23-Paramètres!$B$6*COS(C23)</f>
+        <f>A23-Paramètres!$B$6*COS(C23*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E23" s="1">
-        <f>B23-Paramètres!$B$6*SIN(C23)</f>
+        <f>B23-Paramètres!$B$6*SIN(C23*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1384,15 +1420,15 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
-        <f>A24-Paramètres!$B$6*COS(C24)</f>
+        <f>A24-Paramètres!$B$6*COS(C24*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E24" s="1">
-        <f>B24-Paramètres!$B$6*SIN(C24)</f>
+        <f>B24-Paramètres!$B$6*SIN(C24*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1401,15 +1437,15 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
-        <f>A25-Paramètres!$B$6*COS(C25)</f>
+        <f>A25-Paramètres!$B$6*COS(C25*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E25" s="1">
-        <f>B25-Paramètres!$B$6*SIN(C25)</f>
+        <f>B25-Paramètres!$B$6*SIN(C25*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1418,15 +1454,15 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <f>A26-Paramètres!$B$6*COS(C26)</f>
+        <f>A26-Paramètres!$B$6*COS(C26*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E26" s="1">
-        <f>B26-Paramètres!$B$6*SIN(C26)</f>
+        <f>B26-Paramètres!$B$6*SIN(C26*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1435,15 +1471,15 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
-        <f>A27-Paramètres!$B$6*COS(C27)</f>
+        <f>A27-Paramètres!$B$6*COS(C27*PI()/180 )</f>
         <v>-183</v>
       </c>
       <c r="E27" s="1">
-        <f>B27-Paramètres!$B$6*SIN(C27)</f>
+        <f>B27-Paramètres!$B$6*SIN(C27*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>